<commit_message>
Finished my bad documentation.
</commit_message>
<xml_diff>
--- a/Members.xlsx
+++ b/Members.xlsx
@@ -808,72 +808,6 @@
     <t>vv7</t>
   </si>
   <si>
-    <t>v70</t>
-  </si>
-  <si>
-    <t>v71</t>
-  </si>
-  <si>
-    <t>v72</t>
-  </si>
-  <si>
-    <t>v73</t>
-  </si>
-  <si>
-    <t>v74</t>
-  </si>
-  <si>
-    <t>v75</t>
-  </si>
-  <si>
-    <t>v76</t>
-  </si>
-  <si>
-    <t>v77</t>
-  </si>
-  <si>
-    <t>v78</t>
-  </si>
-  <si>
-    <t>v79</t>
-  </si>
-  <si>
-    <t>v80</t>
-  </si>
-  <si>
-    <t>v81</t>
-  </si>
-  <si>
-    <t>v82</t>
-  </si>
-  <si>
-    <t>v83</t>
-  </si>
-  <si>
-    <t>v84</t>
-  </si>
-  <si>
-    <t>v85</t>
-  </si>
-  <si>
-    <t>v86</t>
-  </si>
-  <si>
-    <t>v87</t>
-  </si>
-  <si>
-    <t>v88</t>
-  </si>
-  <si>
-    <t>v89</t>
-  </si>
-  <si>
-    <t>v90</t>
-  </si>
-  <si>
-    <t>v91</t>
-  </si>
-  <si>
     <t>vv8</t>
   </si>
   <si>
@@ -1058,6 +992,72 @@
   </si>
   <si>
     <t>vv62</t>
+  </si>
+  <si>
+    <t>vv70</t>
+  </si>
+  <si>
+    <t>vv85</t>
+  </si>
+  <si>
+    <t>vv78</t>
+  </si>
+  <si>
+    <t>vv86</t>
+  </si>
+  <si>
+    <t>vv79</t>
+  </si>
+  <si>
+    <t>vv71</t>
+  </si>
+  <si>
+    <t>vv87</t>
+  </si>
+  <si>
+    <t>vv80</t>
+  </si>
+  <si>
+    <t>vv72</t>
+  </si>
+  <si>
+    <t>vv88</t>
+  </si>
+  <si>
+    <t>vv81</t>
+  </si>
+  <si>
+    <t>vv73</t>
+  </si>
+  <si>
+    <t>vv74</t>
+  </si>
+  <si>
+    <t>vv75</t>
+  </si>
+  <si>
+    <t>vv91</t>
+  </si>
+  <si>
+    <t>vv83</t>
+  </si>
+  <si>
+    <t>vv76</t>
+  </si>
+  <si>
+    <t>vv77</t>
+  </si>
+  <si>
+    <t>vv84</t>
+  </si>
+  <si>
+    <t>vv82</t>
+  </si>
+  <si>
+    <t>vv89</t>
+  </si>
+  <si>
+    <t>vv90</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1434,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2510,7 +2510,7 @@
   <dimension ref="A2:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,8 +2804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2997,7 +2997,7 @@
         <v>230</v>
       </c>
       <c r="E11" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -3019,7 +3019,7 @@
         <v>230</v>
       </c>
       <c r="E12" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="4" t="s">
@@ -3040,7 +3040,7 @@
         <v>230</v>
       </c>
       <c r="E13" t="s">
-        <v>285</v>
+        <v>263</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -3062,7 +3062,7 @@
         <v>230</v>
       </c>
       <c r="E14" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
@@ -3084,7 +3084,7 @@
         <v>230</v>
       </c>
       <c r="E15" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="S15" s="4"/>
       <c r="T15" s="4" t="s">
@@ -3105,7 +3105,7 @@
         <v>230</v>
       </c>
       <c r="E16" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="S16" s="4"/>
       <c r="T16" s="4" t="s">
@@ -3126,7 +3126,7 @@
         <v>230</v>
       </c>
       <c r="E17" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
@@ -3148,7 +3148,7 @@
         <v>230</v>
       </c>
       <c r="E18" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="S18" s="4"/>
       <c r="T18" s="4" t="s">
@@ -3169,7 +3169,7 @@
         <v>230</v>
       </c>
       <c r="E19" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
@@ -3191,7 +3191,7 @@
         <v>230</v>
       </c>
       <c r="E20" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
@@ -3211,7 +3211,7 @@
         <v>230</v>
       </c>
       <c r="E21" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -3233,7 +3233,7 @@
         <v>230</v>
       </c>
       <c r="E22" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>230</v>
       </c>
       <c r="E23" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -3267,7 +3267,7 @@
         <v>230</v>
       </c>
       <c r="E24" t="s">
-        <v>299</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -3284,7 +3284,7 @@
         <v>230</v>
       </c>
       <c r="E25" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -3301,7 +3301,7 @@
         <v>230</v>
       </c>
       <c r="E26" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -3318,7 +3318,7 @@
         <v>230</v>
       </c>
       <c r="E27" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -3335,7 +3335,7 @@
         <v>230</v>
       </c>
       <c r="E28" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -3352,7 +3352,7 @@
         <v>230</v>
       </c>
       <c r="E29" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -3369,7 +3369,7 @@
         <v>230</v>
       </c>
       <c r="E30" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -3386,7 +3386,7 @@
         <v>230</v>
       </c>
       <c r="E31" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -3403,7 +3403,7 @@
         <v>230</v>
       </c>
       <c r="E32" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3420,7 +3420,7 @@
         <v>230</v>
       </c>
       <c r="E33" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3437,7 +3437,7 @@
         <v>230</v>
       </c>
       <c r="E34" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3454,7 +3454,7 @@
         <v>230</v>
       </c>
       <c r="E35" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3471,7 +3471,7 @@
         <v>230</v>
       </c>
       <c r="E36" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3488,7 +3488,7 @@
         <v>230</v>
       </c>
       <c r="E37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3505,7 +3505,7 @@
         <v>230</v>
       </c>
       <c r="E38" t="s">
-        <v>310</v>
+        <v>288</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3522,7 +3522,7 @@
         <v>230</v>
       </c>
       <c r="E39" t="s">
-        <v>311</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3539,7 +3539,7 @@
         <v>230</v>
       </c>
       <c r="E40" t="s">
-        <v>312</v>
+        <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3556,7 +3556,7 @@
         <v>230</v>
       </c>
       <c r="E41" t="s">
-        <v>313</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3573,7 +3573,7 @@
         <v>231</v>
       </c>
       <c r="E42" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3590,7 +3590,7 @@
         <v>230</v>
       </c>
       <c r="E43" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3607,7 +3607,7 @@
         <v>230</v>
       </c>
       <c r="E44" t="s">
-        <v>316</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3624,7 +3624,7 @@
         <v>230</v>
       </c>
       <c r="E45" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3641,7 +3641,7 @@
         <v>230</v>
       </c>
       <c r="E46" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3658,7 +3658,7 @@
         <v>230</v>
       </c>
       <c r="E47" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3675,7 +3675,7 @@
         <v>230</v>
       </c>
       <c r="E48" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,7 +3692,7 @@
         <v>231</v>
       </c>
       <c r="E49" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3709,7 +3709,7 @@
         <v>230</v>
       </c>
       <c r="E50" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3726,7 +3726,7 @@
         <v>230</v>
       </c>
       <c r="E51" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3743,7 +3743,7 @@
         <v>230</v>
       </c>
       <c r="E52" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3760,7 +3760,7 @@
         <v>230</v>
       </c>
       <c r="E53" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3777,7 +3777,7 @@
         <v>230</v>
       </c>
       <c r="E54" t="s">
-        <v>326</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3794,7 +3794,7 @@
         <v>230</v>
       </c>
       <c r="E55" t="s">
-        <v>327</v>
+        <v>305</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,7 +3811,7 @@
         <v>230</v>
       </c>
       <c r="E56" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,7 +3828,7 @@
         <v>230</v>
       </c>
       <c r="E57" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3845,7 +3845,7 @@
         <v>230</v>
       </c>
       <c r="E58" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3862,7 +3862,7 @@
         <v>230</v>
       </c>
       <c r="E59" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3879,7 +3879,7 @@
         <v>230</v>
       </c>
       <c r="E60" t="s">
-        <v>333</v>
+        <v>311</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3896,7 +3896,7 @@
         <v>230</v>
       </c>
       <c r="E61" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3913,7 +3913,7 @@
         <v>230</v>
       </c>
       <c r="E62" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3930,7 +3930,7 @@
         <v>230</v>
       </c>
       <c r="E63" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3947,7 +3947,7 @@
         <v>230</v>
       </c>
       <c r="E64" t="s">
-        <v>329</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3964,7 +3964,7 @@
         <v>232</v>
       </c>
       <c r="E65" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3981,7 +3981,7 @@
         <v>230</v>
       </c>
       <c r="E66" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3998,7 +3998,7 @@
         <v>230</v>
       </c>
       <c r="E67" t="s">
-        <v>342</v>
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -4015,7 +4015,7 @@
         <v>230</v>
       </c>
       <c r="E68" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -4032,7 +4032,7 @@
         <v>230</v>
       </c>
       <c r="E69" t="s">
-        <v>340</v>
+        <v>318</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -4049,7 +4049,7 @@
         <v>230</v>
       </c>
       <c r="E70" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -4066,7 +4066,7 @@
         <v>230</v>
       </c>
       <c r="E71" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4083,7 +4083,7 @@
         <v>230</v>
       </c>
       <c r="E72" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -4100,7 +4100,7 @@
         <v>230</v>
       </c>
       <c r="E73" t="s">
-        <v>261</v>
+        <v>323</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4117,7 +4117,7 @@
         <v>230</v>
       </c>
       <c r="E74" t="s">
-        <v>262</v>
+        <v>328</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4134,7 +4134,7 @@
         <v>230</v>
       </c>
       <c r="E75" t="s">
-        <v>263</v>
+        <v>331</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4151,7 +4151,7 @@
         <v>230</v>
       </c>
       <c r="E76" t="s">
-        <v>264</v>
+        <v>334</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -4168,7 +4168,7 @@
         <v>231</v>
       </c>
       <c r="E77" t="s">
-        <v>265</v>
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -4185,7 +4185,7 @@
         <v>230</v>
       </c>
       <c r="E78" t="s">
-        <v>266</v>
+        <v>336</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -4202,7 +4202,7 @@
         <v>230</v>
       </c>
       <c r="E79" t="s">
-        <v>267</v>
+        <v>339</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -4219,7 +4219,7 @@
         <v>230</v>
       </c>
       <c r="E80" t="s">
-        <v>268</v>
+        <v>340</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>230</v>
       </c>
       <c r="E81" t="s">
-        <v>269</v>
+        <v>325</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
         <v>230</v>
       </c>
       <c r="E82" t="s">
-        <v>270</v>
+        <v>327</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -4270,7 +4270,7 @@
         <v>230</v>
       </c>
       <c r="E83" t="s">
-        <v>271</v>
+        <v>330</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4287,7 +4287,7 @@
         <v>230</v>
       </c>
       <c r="E84" t="s">
-        <v>272</v>
+        <v>333</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4304,7 +4304,7 @@
         <v>230</v>
       </c>
       <c r="E85" t="s">
-        <v>273</v>
+        <v>342</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4321,7 +4321,7 @@
         <v>230</v>
       </c>
       <c r="E86" t="s">
-        <v>274</v>
+        <v>338</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4338,7 +4338,7 @@
         <v>230</v>
       </c>
       <c r="E87" t="s">
-        <v>275</v>
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4355,7 +4355,7 @@
         <v>230</v>
       </c>
       <c r="E88" t="s">
-        <v>276</v>
+        <v>324</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4372,7 +4372,7 @@
         <v>230</v>
       </c>
       <c r="E89" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4389,7 +4389,7 @@
         <v>230</v>
       </c>
       <c r="E90" t="s">
-        <v>278</v>
+        <v>329</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -4406,7 +4406,7 @@
         <v>230</v>
       </c>
       <c r="E91" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4423,7 +4423,7 @@
         <v>230</v>
       </c>
       <c r="E92" t="s">
-        <v>280</v>
+        <v>343</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4440,7 +4440,7 @@
         <v>230</v>
       </c>
       <c r="E93" t="s">
-        <v>281</v>
+        <v>344</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -4457,7 +4457,7 @@
         <v>230</v>
       </c>
       <c r="E94" t="s">
-        <v>282</v>
+        <v>337</v>
       </c>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>